<commit_message>
Refactor Excel data handling in dashboard components: Implement API calls for fetching customers, products, and invoices, enhancing error handling and ensuring data integrity. This update improves the user experience by providing a more reliable data management approach across the dashboard.
</commit_message>
<xml_diff>
--- a/data/Customers.xlsx
+++ b/data/Customers.xlsx
@@ -397,13 +397,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>email</v>
+      </c>
+      <c r="C1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="D1" t="str">
+        <v>gstin</v>
+      </c>
+      <c r="E1" t="str">
+        <v>billing_address</v>
+      </c>
+      <c r="F1" t="str">
+        <v>shipping_address</v>
+      </c>
+      <c r="G1" t="str">
+        <v>notes</v>
+      </c>
+      <c r="H1" t="str">
+        <v>id</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Customer QA</v>
+      </c>
+      <c r="B2" t="str">
+        <v>qa@example.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>+911234567890</v>
+      </c>
+      <c r="D2" t="str">
+        <v>GST9901QA</v>
+      </c>
+      <c r="E2" t="str">
+        <v>QATown 1</v>
+      </c>
+      <c r="F2" t="str">
+        <v>QATown 2</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Fake customer (test)</v>
+      </c>
+      <c r="H2" t="str">
+        <v>af892bfb-eb9d-40aa-b377-20bb463398bc</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Hassan mansuri</v>
+      </c>
+      <c r="B3" t="str">
+        <v>hassanmansuri570@gmail.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>+919322909257</v>
+      </c>
+      <c r="D3" t="str">
+        <v>34353</v>
+      </c>
+      <c r="E3" t="str">
+        <v>KPKD</v>
+      </c>
+      <c r="F3" t="str">
+        <v>NAGPUR</v>
+      </c>
+      <c r="G3" t="str">
+        <v>fdghrha</v>
+      </c>
+      <c r="H3" t="str">
+        <v>57fe89c5-a399-4dd1-9830-f513fc466f73</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>gogo</v>
+      </c>
+      <c r="B4" t="str">
+        <v>hassanmansuri570@gmail.com</v>
+      </c>
+      <c r="C4" t="str">
+        <v>+919322909257ee</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>KPKDefe</v>
+      </c>
+      <c r="F4" t="str">
+        <v>NAGPURef</v>
+      </c>
+      <c r="G4" t="str">
+        <v>fdbfbfdb e gh</v>
+      </c>
+      <c r="H4" t="str">
+        <v>6a4f98a3-e2fa-44da-8b37-868632dfbee8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Customer QA</v>
+      </c>
+      <c r="B5" t="str">
+        <v>qa@example.com</v>
+      </c>
+      <c r="C5" t="str">
+        <v>+911234567890</v>
+      </c>
+      <c r="D5" t="str">
+        <v>GST9901QA</v>
+      </c>
+      <c r="E5" t="str">
+        <v>QATown 1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>QATown 2</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Fake customer (test)</v>
+      </c>
+      <c r="H5" t="str">
+        <v>7dd73460-a560-4874-886f-78e863a66d49</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance error handling and logging in dashboard components: Improve data fetching for customers, products, and invoices by adding console logs and user notifications for empty data scenarios. Update manifest to use a placeholder logo for better branding consistency.
</commit_message>
<xml_diff>
--- a/data/Customers.xlsx
+++ b/data/Customers.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>7dd73460-a560-4874-886f-78e863a66d49</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Ha65ssan757 mansuri56357357</v>
+      </c>
+      <c r="B6" t="str">
+        <v>hassanmansuri570@gmail.com</v>
+      </c>
+      <c r="C6" t="str">
+        <v>+919322909257</v>
+      </c>
+      <c r="D6" t="str">
+        <v>w54465</v>
+      </c>
+      <c r="E6" t="str">
+        <v>KPKD653</v>
+      </c>
+      <c r="F6" t="str">
+        <v>NAGPUR65</v>
+      </c>
+      <c r="G6" t="str">
+        <v>thrtj</v>
+      </c>
+      <c r="H6" t="str">
+        <v>b059e276-3c83-4fc3-8b41-2b8e729cfac4</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>